<commit_message>
appended gym numbers, filled gym ratios
</commit_message>
<xml_diff>
--- a/resources/Fitness_Domain_data.xlsx
+++ b/resources/Fitness_Domain_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anna1/Documents/1_career/1_ut_boot_camp/1_local_my/b_homeworks_and_group_projects/class_projects/class-project-1/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE4351-82C8-5640-845A-0E8C5C251836}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903324C3-53CD-ED43-87F8-732F1BAEBE43}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1140" windowWidth="23360" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1040" windowWidth="23360" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="City" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>Metropolitan</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Manhattan - New York County</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spending </t>
   </si>
   <si>
     <t>Detroit</t>
@@ -328,9 +325,6 @@
     <t>Average travel time to work of workers(minutes)</t>
   </si>
   <si>
-    <t>Longtitude</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -359,6 +353,15 @@
   </si>
   <si>
     <t>PA</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Total gyms</t>
+  </si>
+  <si>
+    <t>Total 24h gyms</t>
   </si>
 </sst>
 </file>
@@ -790,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -806,132 +809,149 @@
     <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.83203125" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>97</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>109</v>
+      </c>
+      <c r="P3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>7.67</v>
+      </c>
       <c r="E4" s="16">
         <v>33.847700000000003</v>
       </c>
@@ -956,17 +976,26 @@
       <c r="M4" s="2">
         <v>80365</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>1500</v>
+      </c>
+      <c r="P4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
       <c r="E5" s="16">
         <v>41.928800000000003</v>
       </c>
@@ -991,17 +1020,26 @@
       <c r="M5" s="2">
         <v>79738</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>2300</v>
+      </c>
+      <c r="P5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
       <c r="E6" s="16">
         <v>32.782499999999999</v>
       </c>
@@ -1026,17 +1064,26 @@
       <c r="M6" s="2">
         <v>81574</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>1600</v>
+      </c>
+      <c r="P6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>6.19</v>
+      </c>
       <c r="E7" s="16">
         <v>39.752499999999998</v>
       </c>
@@ -1061,17 +1108,26 @@
       <c r="M7" s="2">
         <v>105447</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>1600</v>
+      </c>
+      <c r="P7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D8">
+        <v>9.76</v>
+      </c>
       <c r="E8" s="16">
         <v>42.367899999999999</v>
       </c>
@@ -1096,16 +1152,25 @@
       <c r="M8" s="2">
         <v>80597</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>717</v>
+      </c>
+      <c r="P8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>3.88</v>
       </c>
       <c r="E9" s="16">
         <v>34.0396</v>
@@ -1131,17 +1196,26 @@
       <c r="M9" s="2">
         <v>76721</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>6600</v>
+      </c>
+      <c r="P9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D10">
+        <v>3.62</v>
+      </c>
       <c r="E10" s="16">
         <v>25.938800000000001</v>
       </c>
@@ -1166,17 +1240,26 @@
       <c r="M10" s="2">
         <v>73843</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>1300</v>
+      </c>
+      <c r="P10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
+      <c r="D11">
+        <v>6.14</v>
+      </c>
       <c r="E11" s="16">
         <v>40.752800000000001</v>
       </c>
@@ -1201,17 +1284,26 @@
       <c r="M11" s="2">
         <v>87106</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>1400</v>
+      </c>
+      <c r="P11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D12">
+        <v>2.94</v>
+      </c>
       <c r="E12" s="16">
         <v>39.952399999999997</v>
       </c>
@@ -1236,26 +1328,50 @@
       <c r="M12" s="2">
         <v>85785</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>5100</v>
+      </c>
+      <c r="P12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1267,7 +1383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
@@ -1296,39 +1412,39 @@
     </row>
     <row r="3" spans="1:10" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="11">
         <v>2000</v>
@@ -1360,22 +1476,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="12">
         <v>80365</v>
@@ -1407,12 +1523,12 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="13">
         <v>46.7</v>
@@ -1444,17 +1560,17 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="13">
         <v>2.6</v>
@@ -1486,7 +1602,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="13">
         <v>0.7</v>
@@ -1518,7 +1634,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="13">
         <v>0.3</v>
@@ -1550,7 +1666,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="13">
         <v>1.3</v>
@@ -1582,7 +1698,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="13">
         <v>1.8</v>
@@ -1614,12 +1730,12 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="14">
         <v>61</v>
@@ -1651,12 +1767,12 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="12">
         <v>58102</v>
@@ -1688,12 +1804,12 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="11">
         <v>5914</v>
@@ -1725,7 +1841,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="11">
         <v>3421</v>
@@ -1757,7 +1873,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="14">
         <v>406</v>
@@ -1789,7 +1905,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="14">
         <v>910</v>
@@ -1821,7 +1937,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="14">
         <v>295</v>
@@ -1853,7 +1969,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="14">
         <v>636</v>
@@ -1885,7 +2001,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="11">
         <v>1175</v>
@@ -1917,7 +2033,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="11">
         <v>2493</v>
@@ -1949,12 +2065,12 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="14">
         <v>297</v>
@@ -1986,12 +2102,12 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="11">
         <v>19811</v>
@@ -2023,7 +2139,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="11">
         <v>11466</v>
@@ -2055,7 +2171,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="11">
         <v>6551</v>
@@ -2087,7 +2203,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="11">
         <v>4043</v>
@@ -2119,7 +2235,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="14">
         <v>873</v>
@@ -2151,7 +2267,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="11">
         <v>4437</v>
@@ -2183,7 +2299,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="11">
         <v>1589</v>
@@ -2215,7 +2331,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="14">
         <v>486</v>
@@ -2247,7 +2363,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="11">
         <v>1833</v>
@@ -2279,12 +2395,12 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="11">
         <v>1892</v>
@@ -2316,12 +2432,12 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="11">
         <v>10649</v>
@@ -2353,7 +2469,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="11">
         <v>5043</v>
@@ -2385,7 +2501,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="11">
         <v>2447</v>
@@ -2417,7 +2533,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="11">
         <v>2647</v>
@@ -2449,7 +2565,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B50" s="14">
         <v>511</v>
@@ -2481,12 +2597,12 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B52" s="11">
         <v>3993</v>
@@ -2518,7 +2634,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="11">
         <v>3061</v>
@@ -2550,7 +2666,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B54" s="14">
         <v>573</v>
@@ -2582,7 +2698,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B55" s="14">
         <v>86</v>
@@ -2614,7 +2730,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B56" s="11">
         <v>1284</v>
@@ -2646,7 +2762,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="14">
         <v>245</v>
@@ -2678,7 +2794,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="14">
         <v>572</v>
@@ -2710,7 +2826,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B59" s="11">
         <v>1702</v>
@@ -2742,12 +2858,12 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61" s="11">
         <v>8022</v>
@@ -2779,7 +2895,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" s="14">
         <v>174</v>
@@ -2811,7 +2927,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" s="11">
         <v>7849</v>
@@ -2843,12 +2959,12 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B65"/>
       <c r="D65"/>
@@ -2856,7 +2972,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -2890,13 +3006,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>